<commit_message>
modified version of results has been uploaded to the word and pdf versions of files called Overall
</commit_message>
<xml_diff>
--- a/Results/Scenario4-TwoSkillsThreeMediumThreeHigh-OneSkillAllLow/ExpertiseBased/WithFigures/TeamStats.xlsx
+++ b/Results/Scenario4-TwoSkillsThreeMediumThreeHigh-OneSkillAllLow/ExpertiseBased/WithFigures/TeamStats.xlsx
@@ -763,11 +763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1569345728"/>
-        <c:axId val="1569353344"/>
+        <c:axId val="350915984"/>
+        <c:axId val="350911632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1569345728"/>
+        <c:axId val="350915984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1569353344"/>
+        <c:crossAx val="350911632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -811,7 +811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1569353344"/>
+        <c:axId val="350911632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1569345728"/>
+        <c:crossAx val="350915984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1009,11 +1009,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1569349536"/>
-        <c:axId val="1569350080"/>
+        <c:axId val="350918704"/>
+        <c:axId val="350912720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1569349536"/>
+        <c:axId val="350918704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1569350080"/>
+        <c:crossAx val="350912720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1057,7 +1057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1569350080"/>
+        <c:axId val="350912720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1068,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1569349536"/>
+        <c:crossAx val="350918704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1393,11 +1393,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1569351712"/>
-        <c:axId val="1569352256"/>
+        <c:axId val="350919248"/>
+        <c:axId val="350922512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1569351712"/>
+        <c:axId val="350919248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1433,7 +1433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1569352256"/>
+        <c:crossAx val="350922512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1441,7 +1441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1569352256"/>
+        <c:axId val="350922512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1479,7 +1479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1569351712"/>
+        <c:crossAx val="350919248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1695,8 +1695,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1598209024"/>
-        <c:axId val="1598210112"/>
+        <c:axId val="350919792"/>
+        <c:axId val="350916528"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1785,11 +1785,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1598194880"/>
-        <c:axId val="1598198688"/>
+        <c:axId val="350913264"/>
+        <c:axId val="350910544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1598209024"/>
+        <c:axId val="350919792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,7 +1825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1598210112"/>
+        <c:crossAx val="350916528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1833,7 +1833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1598210112"/>
+        <c:axId val="350916528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.5"/>
@@ -1859,12 +1859,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1598209024"/>
+        <c:crossAx val="350919792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1598198688"/>
+        <c:axId val="350910544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,12 +1888,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1598194880"/>
+        <c:crossAx val="350913264"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1598194880"/>
+        <c:axId val="350913264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1902,7 +1902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1598198688"/>
+        <c:crossAx val="350910544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>

</xml_diff>